<commit_message>
Updated input file with correct coordinates for Lesotho and eliminated limit on PV nameplate output in Solar calcs
</commit_message>
<xml_diff>
--- a/uGrid/TEST_uGrid_Input.xlsx
+++ b/uGrid/TEST_uGrid_Input.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattmso/Documents/GitHub/uGrid_uGridNet/uGrid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD97B71F-AEC1-9440-86B9-523B85689401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F02ABA6D-079D-814C-9D97-C6E05A4188D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3560" yWindow="760" windowWidth="16380" windowHeight="8200" tabRatio="500" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
     <definedName name="headers">[1]PARTS!$A$1:$AMJ$1</definedName>
     <definedName name="parts">[1]PARTS!$A$3:$AMJ$1432</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterate="1" iterateCount="1" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1355,7 +1355,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="15"/>
@@ -1400,10 +1400,10 @@
         <v>2005</v>
       </c>
       <c r="B2">
-        <v>-33</v>
+        <v>28</v>
       </c>
       <c r="C2">
-        <v>18</v>
+        <v>-29</v>
       </c>
       <c r="D2">
         <v>2</v>

</xml_diff>